<commit_message>
Separated grades and added W/EX
</commit_message>
<xml_diff>
--- a/OBJECTIVES/CS_OBJECTIVES.xlsx
+++ b/OBJECTIVES/CS_OBJECTIVES.xlsx
@@ -5,22 +5,34 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\REALE\SUNYIT\Tools\AssessmentGenerator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\REALE\SUNYIT\Tools\AssessmentGenerator\OBJECTIVES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F1494F4-933B-4FA6-A4B5-731C108C5F24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54D4AF55-253D-4006-959D-F59E663D1488}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OBJECTIVES" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="66">
   <si>
     <t>Student learning Outcome/Performance Indicator</t>
   </si>
@@ -316,6 +328,9 @@
   </si>
   <si>
     <t>Count Meeting Outcome</t>
+  </si>
+  <si>
+    <t>W and EX Count</t>
   </si>
 </sst>
 </file>
@@ -1159,21 +1174,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J37"/>
+  <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="8.7265625" style="1"/>
-    <col min="4" max="4" width="47.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="76.1796875" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="3" width="8.7109375" style="1"/>
+    <col min="4" max="4" width="47.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="76.140625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>56</v>
       </c>
@@ -1196,16 +1211,19 @@
         <v>64</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>60</v>
       </c>
@@ -1222,7 +1240,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>60</v>
       </c>
@@ -1239,7 +1257,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="116" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>60</v>
       </c>
@@ -1256,7 +1274,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>60</v>
       </c>
@@ -1273,7 +1291,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>60</v>
       </c>
@@ -1290,7 +1308,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>60</v>
       </c>
@@ -1307,7 +1325,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>60</v>
       </c>
@@ -1324,7 +1342,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>60</v>
       </c>
@@ -1341,7 +1359,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>60</v>
       </c>
@@ -1358,7 +1376,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>60</v>
       </c>
@@ -1375,7 +1393,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>60</v>
       </c>
@@ -1392,7 +1410,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>60</v>
       </c>
@@ -1409,7 +1427,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>60</v>
       </c>
@@ -1426,7 +1444,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>60</v>
       </c>
@@ -1443,7 +1461,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>60</v>
       </c>
@@ -1460,7 +1478,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>60</v>
       </c>
@@ -1477,7 +1495,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>60</v>
       </c>
@@ -1494,7 +1512,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>60</v>
       </c>
@@ -1511,7 +1529,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>60</v>
       </c>
@@ -1528,7 +1546,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>60</v>
       </c>
@@ -1545,7 +1563,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>60</v>
       </c>
@@ -1562,7 +1580,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>60</v>
       </c>
@@ -1579,7 +1597,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" ht="210" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>60</v>
       </c>
@@ -1596,7 +1614,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>60</v>
       </c>
@@ -1613,7 +1631,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="377" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" ht="390" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>60</v>
       </c>
@@ -1630,7 +1648,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="116" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>60</v>
       </c>
@@ -1647,7 +1665,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="203" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" ht="210" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>60</v>
       </c>
@@ -1664,7 +1682,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="246.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" ht="255" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>60</v>
       </c>
@@ -1681,7 +1699,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>60</v>
       </c>
@@ -1698,7 +1716,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>60</v>
       </c>
@@ -1715,7 +1733,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>61</v>
       </c>
@@ -1732,7 +1750,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>61</v>
       </c>
@@ -1749,7 +1767,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>61</v>
       </c>
@@ -1766,7 +1784,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>61</v>
       </c>
@@ -1783,7 +1801,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>61</v>
       </c>
@@ -1800,7 +1818,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>61</v>
       </c>
@@ -1818,7 +1836,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J37">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K37">
     <sortCondition ref="A2:A37"/>
     <sortCondition ref="B2:B37"/>
     <sortCondition ref="C2:C37"/>

</xml_diff>

<commit_message>
Changed CS objectives to include I/IP in exclusion
</commit_message>
<xml_diff>
--- a/OBJECTIVES/CS_OBJECTIVES.xlsx
+++ b/OBJECTIVES/CS_OBJECTIVES.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\REALE\SUNYIT\Tools\AssessmentGenerator\OBJECTIVES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54D4AF55-253D-4006-959D-F59E663D1488}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BE42884-99A2-48B1-90FC-6539B8345DF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OBJECTIVES" sheetId="1" r:id="rId1"/>
@@ -330,14 +330,14 @@
     <t>Count Meeting Outcome</t>
   </si>
   <si>
-    <t>W and EX Count</t>
+    <t>W, I, IP, EX Count</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -468,6 +468,13 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF444444"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -814,9 +821,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1" shrinkToFit="1"/>
     </xf>
   </cellXfs>
@@ -1210,7 +1220,7 @@
       <c r="G1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>65</v>
       </c>
       <c r="I1" s="1" t="s">

</xml_diff>

<commit_message>
Auto-grade extraction and W/I/IP/EX included
</commit_message>
<xml_diff>
--- a/OBJECTIVES/CS_OBJECTIVES.xlsx
+++ b/OBJECTIVES/CS_OBJECTIVES.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\REALE\SUNYIT\Tools\AssessmentGenerator\OBJECTIVES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BE42884-99A2-48B1-90FC-6539B8345DF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D8C1A76-FC25-4959-AE1A-9235BFBE4C1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OBJECTIVES" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="65">
   <si>
     <t>Student learning Outcome/Performance Indicator</t>
   </si>
@@ -329,15 +329,12 @@
   <si>
     <t>Count Meeting Outcome</t>
   </si>
-  <si>
-    <t>W, I, IP, EX Count</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -468,13 +465,6 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF444444"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -821,12 +811,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1" shrinkToFit="1"/>
     </xf>
   </cellXfs>
@@ -1184,10 +1171,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K37"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1198,7 +1185,7 @@
     <col min="6" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>56</v>
       </c>
@@ -1220,20 +1207,17 @@
       <c r="G1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>65</v>
+      <c r="H1" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>60</v>
       </c>
@@ -1250,7 +1234,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>60</v>
       </c>
@@ -1267,7 +1251,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>60</v>
       </c>
@@ -1284,7 +1268,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>60</v>
       </c>
@@ -1301,7 +1285,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>60</v>
       </c>
@@ -1318,7 +1302,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>60</v>
       </c>
@@ -1335,7 +1319,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>60</v>
       </c>
@@ -1352,7 +1336,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>60</v>
       </c>
@@ -1369,7 +1353,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>60</v>
       </c>
@@ -1386,7 +1370,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>60</v>
       </c>
@@ -1403,7 +1387,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>60</v>
       </c>
@@ -1420,7 +1404,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>60</v>
       </c>
@@ -1437,7 +1421,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>60</v>
       </c>
@@ -1454,7 +1438,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>60</v>
       </c>
@@ -1471,7 +1455,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>60</v>
       </c>
@@ -1846,7 +1830,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K37">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J37">
     <sortCondition ref="A2:A37"/>
     <sortCondition ref="B2:B37"/>
     <sortCondition ref="C2:C37"/>

</xml_diff>